<commit_message>
Cam - full read through and edits
</commit_message>
<xml_diff>
--- a/data_examples/metadata_data_example.xlsx
+++ b/data_examples/metadata_data_example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_projects\stats-production-guidance\data_examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08D91ED-B644-46B4-9070-1FECF878DC59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B943C616-CDE1-42E9-947F-67053F25C2C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>…</t>
+  </si>
+  <si>
+    <t>gender</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,13 +411,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -434,7 +434,7 @@
         <v>2018</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -443,7 +443,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2">
         <v>240</v>
@@ -457,16 +457,16 @@
         <v>2018</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>200</v>
@@ -480,16 +480,16 @@
         <v>2018</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
       </c>
       <c r="F4">
         <v>440</v>
@@ -503,7 +503,7 @@
         <v>2018</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -512,7 +512,7 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>240</v>
@@ -526,16 +526,16 @@
         <v>2018</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>220</v>
@@ -549,16 +549,16 @@
         <v>2018</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7">
         <v>460</v>
@@ -572,7 +572,7 @@
         <v>2018</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -581,7 +581,7 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <v>480</v>
@@ -595,16 +595,16 @@
         <v>2018</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
         <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
       </c>
       <c r="F9">
         <v>420</v>
@@ -618,16 +618,16 @@
         <v>2018</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <v>900</v>

</xml_diff>